<commit_message>
Revert "Correct file extension"
This reverts commit 9637ebd57ff1a44adb7e5bcd8a2b8be405d428d4.
</commit_message>
<xml_diff>
--- a/USR_FILES/VENTAS/Colores.xlsx
+++ b/USR_FILES/VENTAS/Colores.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7032"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -240,7 +240,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -529,15 +529,15 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D2" sqref="D2:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -551,7 +551,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,7 +565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -576,10 +576,10 @@
         <v>230</v>
       </c>
       <c r="D3" s="6">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -593,7 +593,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -607,7 +607,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -621,7 +621,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -635,7 +635,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -649,7 +649,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -663,7 +663,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -677,7 +677,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>

</xml_diff>